<commit_message>
update to 1376 columns
</commit_message>
<xml_diff>
--- a/data/input/Banco de dados_final_0708.xlsx
+++ b/data/input/Banco de dados_final_0708.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kelsonthony/Dev/projects/trajectory-analysis/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1337DF-1FDD-8E46-89FF-817F20C6F0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49917F8-28DF-074A-9AA9-CF6E1AC899CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9820" yWindow="660" windowWidth="41380" windowHeight="19240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RTrajet" sheetId="2" r:id="rId1"/>
@@ -115,11 +115,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="165" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="168" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="169" formatCode="dd\-mm\-yyyy"/>
+    <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="167" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="168" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -133,22 +133,26 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -338,19 +342,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -359,7 +363,19 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -368,80 +384,68 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -453,44 +457,44 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -502,49 +506,49 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -767,9 +771,9 @@
   </sheetPr>
   <dimension ref="A1:U1383"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A719" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A730" sqref="A730"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5764,7 +5768,7 @@
     </row>
     <row r="130" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A130" s="7">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B130" s="8" t="s">
         <v>2</v>
@@ -29533,7 +29537,7 @@
     </row>
     <row r="727" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A727" s="4">
-        <v>736</v>
+        <v>726</v>
       </c>
       <c r="B727" s="8" t="s">
         <v>1</v>

</xml_diff>